<commit_message>
Updating Fact mapping specs
</commit_message>
<xml_diff>
--- a/Mapping Spec Git.xlsx
+++ b/Mapping Spec Git.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt.wilkinson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jsainsbury-my.sharepoint.com/personal/matt_wilkinson_sainsburys_co_uk/Documents/Documents/GitHub/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF5A895-E28E-8348-915D-BE64AF5917C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{AEF5A895-E28E-8348-915D-BE64AF5917C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5689961D-F6E4-1043-9E81-696FD8718C69}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{0DC20B23-C7A0-FB40-BE05-8EE6DBDC62EA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{0DC20B23-C7A0-FB40-BE05-8EE6DBDC62EA}"/>
   </bookViews>
   <sheets>
     <sheet name="New Markdown Format" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="168">
   <si>
     <t>Source System</t>
   </si>
@@ -486,18 +486,12 @@
     <t>AGG_ITEM_SPECIFICATION_COMPONENT</t>
   </si>
   <si>
-    <t>sum</t>
-  </si>
-  <si>
     <t>ITEM_WEIGHT</t>
   </si>
   <si>
     <t>ITEM_RECYCLED_WEIGHT</t>
   </si>
   <si>
-    <t>recycled_weight/component_weight</t>
-  </si>
-  <si>
     <t>RECYCLABILITY_PCT</t>
   </si>
   <si>
@@ -553,6 +547,15 @@
   </si>
   <si>
     <t>Setup with Mithra</t>
+  </si>
+  <si>
+    <t>Total Tonnage(with Recycling_Advice_Icon filtered/Total Tonnage</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Recycled_Weight/Component_Weight</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -831,17 +834,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -878,14 +870,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -910,6 +895,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1281,7 +1287,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1327,10 +1333,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="44">
+      <c r="A2" s="36">
         <v>1</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="36" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1340,7 +1346,7 @@
         <v>77</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>115</v>
@@ -1352,7 +1358,7 @@
         <v>45037</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1375,60 +1381,60 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="37">
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="37" t="s">
         <v>78</v>
       </c>
       <c r="F4" s="11"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16" t="s">
-        <v>158</v>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="A6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="44">
+      <c r="A7" s="36">
         <v>4</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="36" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -1438,7 +1444,7 @@
         <v>81</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>115</v>
@@ -1479,20 +1485,20 @@
       <c r="B9" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="37" t="s">
         <v>78</v>
       </c>
       <c r="F9" s="11"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16" t="s">
-        <v>159</v>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1502,13 +1508,13 @@
       <c r="B10" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
@@ -1527,12 +1533,12 @@
         <v>78</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1557,7 +1563,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,7 +1588,7 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1607,7 +1613,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1628,38 +1634,38 @@
       <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
+      <c r="A16" s="37">
         <v>12</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="37" t="s">
         <v>78</v>
       </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16" t="s">
-        <v>165</v>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
@@ -1683,7 +1689,7 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1703,7 +1709,7 @@
         <v>78</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -1729,7 +1735,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1772,7 +1778,7 @@
         <v>78</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -1819,6 +1825,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="C4:C6"/>
@@ -1832,14 +1846,6 @@
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://sainsburys-confluence.valiantys.net/display/~sandeep.patil1" xr:uid="{DD1145ED-45AE-3D4B-A0FA-83AC83BD89EB}"/>
@@ -1867,7 +1873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B998930-761E-0740-A8E1-3177EC5D4273}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -2138,10 +2144,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2158,13 +2164,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="16" t="s">
         <v>137</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2178,13 +2184,13 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="17" t="s">
         <v>138</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2407,309 +2413,317 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="75" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="F1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="G1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="30" t="s">
+      <c r="A2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="B3" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="B4" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="29" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="B6" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="29" t="s">
+      <c r="C6" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="B7" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="29" t="s">
+      <c r="C7" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="B8" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="G6" s="29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="29" t="s">
+      <c r="C8" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="B9" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="G7" s="29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="29" t="s">
+      <c r="C9" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="B10" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="C10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="42" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>148</v>
+      <c r="D13" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2721,361 +2735,361 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50F088E-367F-9940-B1EA-EF14007FEB5D}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="80" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="F1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="G1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="40" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="D8" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="40" t="s">
+      <c r="B9" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" s="42" t="s">
+      <c r="B10" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="42" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" s="42" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="40" t="s">
+      <c r="B11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G5" s="40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="40" t="s">
+      <c r="B12" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G6" s="40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="40" t="s">
+      <c r="B13" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="40" t="s">
+      <c r="B14" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G9" s="40" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G10" s="40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G14" s="40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="40" t="s">
+      <c r="B15" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="G15" s="40" t="s">
+      <c r="D15" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="32" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3104,45 +3118,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">

</xml_diff>